<commit_message>
Add new armor attibutes.
</commit_message>
<xml_diff>
--- a/attributes_by_armor_Template.xlsx
+++ b/attributes_by_armor_Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>armor_number</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>attribute</t>
+  </si>
+  <si>
+    <t>raw_value</t>
   </si>
 </sst>
 </file>
@@ -384,20 +387,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,6 +409,9 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>